<commit_message>
Add inventories for ammonia
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-ammonia.xlsx
+++ b/premise/data/additional_inventories/lci-ammonia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748189C3-FB69-3D48-8218-7D6D666D0604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057D87EE-32CA-DA48-9318-568311219DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="760" windowWidth="24940" windowHeight="18880" xr2:uid="{65ACB5C6-9A71-F043-B1B5-919D021F4A57}"/>
   </bookViews>
@@ -1478,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263A38E-0BDC-2843-B92F-206445D00D40}">
   <dimension ref="A1:M376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
+      <selection activeCell="B353" sqref="B353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix issue when downloading inventories from data packages
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-ammonia.xlsx
+++ b/premise/data/additional_inventories/lci-ammonia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283A3135-4E18-9443-B88B-77E929FFA484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDE9D5F-B959-D743-A071-E0F3A0D9069E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="760" windowWidth="24940" windowHeight="18880" xr2:uid="{65ACB5C6-9A71-F043-B1B5-919D021F4A57}"/>
   </bookViews>
@@ -1101,9 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1481,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263A38E-0BDC-2843-B92F-206445D00D40}">
   <dimension ref="A1:M376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="A356" sqref="A356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4756,7 +4754,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>3</v>
       </c>

</xml_diff>